<commit_message>
Moving around excel files
</commit_message>
<xml_diff>
--- a/RPi/controllerInterface/ps4ButtonMapping.xlsx
+++ b/RPi/controllerInterface/ps4ButtonMapping.xlsx
@@ -13,7 +13,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -385,7 +385,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -396,6 +396,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -418,7 +422,7 @@
   <dimension ref="A6:C62"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -555,7 +559,7 @@
       <c r="B24" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -566,6 +570,7 @@
       <c r="B25" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="C25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
@@ -574,6 +579,7 @@
       <c r="B26" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="C26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
@@ -582,6 +588,7 @@
       <c r="B27" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="C27" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
@@ -829,12 +836,15 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C24:C27"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>